<commit_message>
woah more fittings stuff cool
</commit_message>
<xml_diff>
--- a/Performance Testing/Fittings_level_tmp.xlsx
+++ b/Performance Testing/Fittings_level_tmp.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\khensu\Home02\froeh\Desktop\GitHub\electric-feed-system\Performance Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnn\Dropbox\GitHub\electric-feed-system\Performance Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -251,7 +251,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="[$$]#,##0.00"/>
@@ -478,6 +478,15 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -490,20 +499,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -788,26 +788,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" customWidth="1"/>
-    <col min="5" max="5" width="56.5703125" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="1" max="2" width="0" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1328125" customWidth="1"/>
+    <col min="4" max="4" width="5.59765625" customWidth="1"/>
+    <col min="5" max="5" width="56.59765625" customWidth="1"/>
+    <col min="6" max="6" width="9.1328125" customWidth="1"/>
+    <col min="7" max="7" width="13.3984375" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" customWidth="1"/>
-    <col min="12" max="12" width="73.7109375" customWidth="1"/>
-    <col min="13" max="13" width="104.140625" customWidth="1"/>
+    <col min="9" max="9" width="16.73046875" customWidth="1"/>
+    <col min="10" max="10" width="15.3984375" customWidth="1"/>
+    <col min="12" max="12" width="73.73046875" customWidth="1"/>
+    <col min="13" max="13" width="104.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="3:13" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="3:13" ht="14.65" hidden="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="3:13" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="3" t="s">
@@ -836,7 +837,7 @@
       </c>
       <c r="M2" s="18"/>
     </row>
-    <row r="3" spans="3:13" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:13" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C3" s="23" t="s">
         <v>0</v>
       </c>
@@ -870,8 +871,8 @@
       </c>
       <c r="M3" s="18"/>
     </row>
-    <row r="4" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="29" t="s">
+    <row r="4" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C4" s="31" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="6">
@@ -906,8 +907,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="29"/>
+    <row r="5" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C5" s="31"/>
       <c r="D5" s="6">
         <v>3</v>
       </c>
@@ -940,8 +941,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="29"/>
+    <row r="6" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C6" s="31"/>
       <c r="D6" s="6">
         <v>4</v>
       </c>
@@ -972,8 +973,8 @@
       </c>
       <c r="M6" s="18"/>
     </row>
-    <row r="7" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="29"/>
+    <row r="7" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C7" s="31"/>
       <c r="D7" s="6">
         <v>5</v>
       </c>
@@ -1004,8 +1005,8 @@
       </c>
       <c r="M7" s="18"/>
     </row>
-    <row r="8" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="27" t="s">
+    <row r="8" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C8" s="30" t="s">
         <v>28</v>
       </c>
       <c r="D8" s="6">
@@ -1040,8 +1041,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="27"/>
+    <row r="9" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C9" s="30"/>
       <c r="D9" s="6">
         <v>7</v>
       </c>
@@ -1072,8 +1073,8 @@
       </c>
       <c r="M9" s="14"/>
     </row>
-    <row r="10" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="27"/>
+    <row r="10" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C10" s="30"/>
       <c r="D10" s="6">
         <v>8</v>
       </c>
@@ -1104,8 +1105,8 @@
       </c>
       <c r="M10" s="18"/>
     </row>
-    <row r="11" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="27"/>
+    <row r="11" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C11" s="30"/>
       <c r="D11" s="6">
         <v>9</v>
       </c>
@@ -1136,7 +1137,7 @@
       </c>
       <c r="M11" s="18"/>
     </row>
-    <row r="12" spans="3:13" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:13" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C12" s="22" t="s">
         <v>32</v>
       </c>
@@ -1172,8 +1173,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="27" t="s">
+    <row r="13" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C13" s="30" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="6">
@@ -1208,8 +1209,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="27"/>
+    <row r="14" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C14" s="30"/>
       <c r="D14" s="6">
         <v>12</v>
       </c>
@@ -1240,8 +1241,8 @@
       </c>
       <c r="M14" s="18"/>
     </row>
-    <row r="15" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="28" t="s">
+    <row r="15" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C15" s="32" t="s">
         <v>36</v>
       </c>
       <c r="D15" s="6">
@@ -1262,8 +1263,8 @@
       <c r="L15" s="10"/>
       <c r="M15" s="18"/>
     </row>
-    <row r="16" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="28"/>
+    <row r="16" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C16" s="32"/>
       <c r="D16" s="6">
         <v>14</v>
       </c>
@@ -1282,11 +1283,11 @@
       <c r="L16" s="10"/>
       <c r="M16" s="18"/>
     </row>
-    <row r="17" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="27" t="s">
+    <row r="17" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C17" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="30">
+      <c r="D17" s="24">
         <v>15</v>
       </c>
       <c r="E17" s="7" t="s">
@@ -1316,8 +1317,8 @@
       </c>
       <c r="M17" s="18"/>
     </row>
-    <row r="18" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="27"/>
+    <row r="18" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C18" s="30"/>
       <c r="D18" s="6">
         <v>16</v>
       </c>
@@ -1348,8 +1349,8 @@
       </c>
       <c r="M18" s="18"/>
     </row>
-    <row r="19" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="27"/>
+    <row r="19" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C19" s="30"/>
       <c r="D19" s="6">
         <v>17</v>
       </c>
@@ -1380,8 +1381,8 @@
       </c>
       <c r="M19" s="18"/>
     </row>
-    <row r="20" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="24" t="s">
+    <row r="20" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C20" s="27" t="s">
         <v>72</v>
       </c>
       <c r="D20" s="6">
@@ -1414,8 +1415,8 @@
       </c>
       <c r="M20" s="18"/>
     </row>
-    <row r="21" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="25"/>
+    <row r="21" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C21" s="28"/>
       <c r="D21" s="6">
         <v>19</v>
       </c>
@@ -1446,9 +1447,9 @@
       </c>
       <c r="M21" s="18"/>
     </row>
-    <row r="22" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="26"/>
-      <c r="D22" s="30">
+    <row r="22" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C22" s="29"/>
+      <c r="D22" s="24">
         <v>20</v>
       </c>
       <c r="E22" s="15" t="s">
@@ -1478,15 +1479,15 @@
       </c>
       <c r="M22" s="18"/>
     </row>
-    <row r="23" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
-      <c r="G23" s="31" t="s">
+      <c r="G23" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="H23" s="32">
+      <c r="H23" s="26">
         <f>SUM(H3:H22)</f>
         <v>484.68</v>
       </c>
@@ -1496,7 +1497,7 @@
       <c r="L23" s="10"/>
       <c r="M23" s="2"/>
     </row>
-    <row r="24" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:13" x14ac:dyDescent="0.45">
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -1506,7 +1507,7 @@
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:13" x14ac:dyDescent="0.45">
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -1516,7 +1517,7 @@
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:13" x14ac:dyDescent="0.45">
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -1526,7 +1527,7 @@
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:13" x14ac:dyDescent="0.45">
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
@@ -1538,7 +1539,7 @@
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:13" x14ac:dyDescent="0.45">
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -1548,7 +1549,7 @@
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
     </row>
-    <row r="29" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:13" x14ac:dyDescent="0.45">
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>

</xml_diff>

<commit_message>
Updated fittings oder and added raw stock to active BOM
</commit_message>
<xml_diff>
--- a/Performance Testing/Fittings_level_tmp.xlsx
+++ b/Performance Testing/Fittings_level_tmp.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnn\Dropbox\GitHub\electric-feed-system\Performance Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John Froehlich\Dropbox\GitHub\electric-feed-system\Performance Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="90">
   <si>
     <t>Suction Valve</t>
   </si>
@@ -246,17 +246,66 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Water Tank</t>
+  </si>
+  <si>
+    <t>MISC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flanged sleeve bushing, Rulon, 5/8" ID, </t>
+  </si>
+  <si>
+    <t>6362K307</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#6362k307/=17999fj</t>
+  </si>
+  <si>
+    <t>1/8" Mill Diameter, 3/8" Shank Diameter, 2-5/16" Overall Length</t>
+  </si>
+  <si>
+    <t>8838A11</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#8838a11/=17e9re4</t>
+  </si>
+  <si>
+    <t>TiAlN Coated High-Speed Steel Two-Flute End Mill</t>
+  </si>
+  <si>
+    <t>5/16" Mill Diameter, 3/8" Shank Diameter, 3/4" Length of Cut</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#8838a826/=17e9t3m</t>
+  </si>
+  <si>
+    <t>8838A826</t>
+  </si>
+  <si>
+    <t>Trade No. 6210, for 50 mm Shaft Diameter, 90 mm OD</t>
+  </si>
+  <si>
+    <t>5972K129</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/#5972k129/=17e9tjt</t>
+  </si>
+  <si>
+    <t>Ball Bearing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="[$$]#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="\$#,##0.00"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,13 +314,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -308,6 +350,25 @@
     <font>
       <sz val="11"/>
       <color rgb="FF222222"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -371,57 +432,57 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left/>
+      <right/>
+      <top style="medium">
         <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -463,19 +524,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -484,29 +539,72 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -786,808 +884,1014 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:M29"/>
+  <dimension ref="C1:M37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="0" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1328125" customWidth="1"/>
-    <col min="4" max="4" width="5.59765625" customWidth="1"/>
-    <col min="5" max="5" width="56.59765625" customWidth="1"/>
-    <col min="6" max="6" width="9.1328125" customWidth="1"/>
-    <col min="7" max="7" width="13.3984375" customWidth="1"/>
-    <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="16.73046875" customWidth="1"/>
-    <col min="10" max="10" width="15.3984375" customWidth="1"/>
-    <col min="12" max="12" width="73.73046875" customWidth="1"/>
-    <col min="13" max="13" width="104.1328125" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" customWidth="1"/>
+    <col min="5" max="5" width="56.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" customWidth="1"/>
+    <col min="12" max="12" width="65.28515625" customWidth="1"/>
+    <col min="13" max="13" width="104.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:13" ht="14.65" hidden="1" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="2" spans="3:13" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="3" t="s">
+    <row r="1" spans="3:13" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="3:13" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="36"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="18"/>
-    </row>
-    <row r="3" spans="3:13" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C3" s="23" t="s">
+      <c r="M3" s="17"/>
+    </row>
+    <row r="4" spans="3:13" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="6">
-        <v>1</v>
-      </c>
-      <c r="E3" s="7" t="s">
+      <c r="D4" s="5">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F4" s="7">
         <v>10.57</v>
       </c>
-      <c r="G3" s="9">
-        <v>1</v>
-      </c>
-      <c r="H3" s="8">
-        <f>F3*G3</f>
+      <c r="G4" s="8">
+        <v>1</v>
+      </c>
+      <c r="H4" s="7">
+        <f>F4*G4</f>
         <v>10.57</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L3" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="M3" s="18"/>
-    </row>
-    <row r="4" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C4" s="31" t="s">
+      <c r="K4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" s="17"/>
+    </row>
+    <row r="5" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D5" s="5">
         <v>2</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F5" s="11">
         <v>73.180000000000007</v>
       </c>
-      <c r="G4" s="13">
-        <v>1</v>
-      </c>
-      <c r="H4" s="12">
-        <f t="shared" ref="H4:H8" si="0">F4*G4</f>
+      <c r="G5" s="12">
+        <v>1</v>
+      </c>
+      <c r="H5" s="11">
+        <f t="shared" ref="H5:H9" si="0">F5*G5</f>
         <v>73.180000000000007</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I5" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="L4" s="19" t="s">
+      <c r="K5" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="M4" s="14" t="s">
+      <c r="M5" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C5" s="31"/>
-      <c r="D5" s="6">
+    <row r="6" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="24"/>
+      <c r="D6" s="5">
         <v>3</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E6" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F6" s="11">
         <v>17.399999999999999</v>
       </c>
-      <c r="G5" s="13">
-        <v>1</v>
-      </c>
-      <c r="H5" s="12">
+      <c r="G6" s="12">
+        <v>1</v>
+      </c>
+      <c r="H6" s="11">
         <f t="shared" si="0"/>
         <v>17.399999999999999</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="I6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="J6" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="L5" s="20" t="s">
+      <c r="K6" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="M5" s="14" t="s">
+      <c r="M6" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C6" s="31"/>
-      <c r="D6" s="6">
+    <row r="7" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="24"/>
+      <c r="D7" s="5">
         <v>4</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E7" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F7" s="11">
         <v>49.39</v>
       </c>
-      <c r="G6" s="13">
-        <v>1</v>
-      </c>
-      <c r="H6" s="12">
+      <c r="G7" s="12">
+        <v>1</v>
+      </c>
+      <c r="H7" s="11">
         <f t="shared" si="0"/>
         <v>49.39</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="J7" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="K6" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="L6" s="20" t="s">
+      <c r="K7" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="M6" s="18"/>
-    </row>
-    <row r="7" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C7" s="31"/>
-      <c r="D7" s="6">
+      <c r="M7" s="17"/>
+    </row>
+    <row r="8" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="24"/>
+      <c r="D8" s="5">
         <v>5</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E8" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F8" s="11">
         <v>2.54</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G8" s="12">
         <v>2</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H8" s="11">
         <f t="shared" si="0"/>
         <v>5.08</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I8" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="J8" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="K7" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="L7" s="20" t="s">
+      <c r="K8" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="M7" s="18"/>
-    </row>
-    <row r="8" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C8" s="30" t="s">
+      <c r="M8" s="17"/>
+    </row>
+    <row r="9" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D9" s="5">
         <v>6</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E9" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F9" s="7">
         <v>18.95</v>
       </c>
-      <c r="G8" s="9">
-        <v>1</v>
-      </c>
-      <c r="H8" s="8">
+      <c r="G9" s="8">
+        <v>1</v>
+      </c>
+      <c r="H9" s="7">
         <f t="shared" si="0"/>
         <v>18.95</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="J9" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="K8" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L8" s="20" t="s">
+      <c r="K9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="M8" s="18" t="s">
+      <c r="M9" s="17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C9" s="30"/>
-      <c r="D9" s="6">
+    <row r="10" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="42"/>
+      <c r="D10" s="5">
         <v>7</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E10" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F10" s="7">
         <v>73.180000000000007</v>
       </c>
-      <c r="G9" s="9">
-        <v>1</v>
-      </c>
-      <c r="H9" s="8">
-        <f t="shared" ref="H9:H22" si="1">F9*G9</f>
+      <c r="G10" s="8">
+        <v>1</v>
+      </c>
+      <c r="H10" s="7">
+        <f t="shared" ref="H10:H30" si="1">F10*G10</f>
         <v>73.180000000000007</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="J10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L9" s="19" t="s">
+      <c r="K10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="M9" s="14"/>
-    </row>
-    <row r="10" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C10" s="30"/>
-      <c r="D10" s="6">
+      <c r="M10" s="13"/>
+    </row>
+    <row r="11" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="42"/>
+      <c r="D11" s="5">
         <v>8</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F11" s="7">
         <v>2.81</v>
       </c>
-      <c r="G10" s="9">
-        <v>1</v>
-      </c>
-      <c r="H10" s="8">
+      <c r="G11" s="8">
+        <v>1</v>
+      </c>
+      <c r="H11" s="7">
         <f t="shared" si="1"/>
         <v>2.81</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J10" s="9" t="s">
+      <c r="J11" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="K10" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L10" s="20" t="s">
+      <c r="K11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="M10" s="18"/>
-    </row>
-    <row r="11" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C11" s="30"/>
-      <c r="D11" s="6">
+      <c r="M11" s="17"/>
+    </row>
+    <row r="12" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="42"/>
+      <c r="D12" s="5">
         <v>9</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E12" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F12" s="7">
         <v>3.69</v>
       </c>
-      <c r="G11" s="9">
-        <v>1</v>
-      </c>
-      <c r="H11" s="8">
+      <c r="G12" s="8">
+        <v>1</v>
+      </c>
+      <c r="H12" s="7">
         <f t="shared" si="1"/>
         <v>3.69</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="I12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="9" t="s">
+      <c r="J12" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="K11" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L11" s="20" t="s">
+      <c r="K12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L12" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="M11" s="18"/>
-    </row>
-    <row r="12" spans="3:13" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C12" s="22" t="s">
+      <c r="M12" s="17"/>
+    </row>
+    <row r="13" spans="3:13" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D13" s="5">
         <v>10</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E13" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F13" s="11">
         <v>15.32</v>
       </c>
-      <c r="G12" s="13">
-        <v>1</v>
-      </c>
-      <c r="H12" s="12">
+      <c r="G13" s="12">
+        <v>1</v>
+      </c>
+      <c r="H13" s="11">
         <f t="shared" si="1"/>
         <v>15.32</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="I13" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="J12" s="21" t="s">
+      <c r="J13" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="K12" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="L12" s="20" t="s">
+      <c r="K13" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="L13" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="M12" s="18" t="s">
+      <c r="M13" s="17" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C13" s="30" t="s">
+    <row r="14" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D14" s="5">
         <v>11</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E14" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F14" s="7">
         <v>56.31</v>
       </c>
-      <c r="G13" s="9">
-        <v>1</v>
-      </c>
-      <c r="H13" s="8">
+      <c r="G14" s="8">
+        <v>1</v>
+      </c>
+      <c r="H14" s="7">
         <f t="shared" si="1"/>
         <v>56.31</v>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="I14" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J13" s="9" t="s">
+      <c r="J14" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="K13" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L13" s="20" t="s">
+      <c r="K14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L14" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="M13" s="18" t="s">
+      <c r="M14" s="17" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C14" s="30"/>
-      <c r="D14" s="6">
+    <row r="15" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="42"/>
+      <c r="D15" s="5">
         <v>12</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E15" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F15" s="7">
         <v>17.399999999999999</v>
       </c>
-      <c r="G14" s="9">
-        <v>1</v>
-      </c>
-      <c r="H14" s="8">
+      <c r="G15" s="8">
+        <v>1</v>
+      </c>
+      <c r="H15" s="7">
         <f t="shared" si="1"/>
         <v>17.399999999999999</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="I15" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J14" s="9" t="s">
+      <c r="J15" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="K14" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L14" s="20" t="s">
+      <c r="K15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L15" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="M14" s="18"/>
-    </row>
-    <row r="15" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C15" s="32" t="s">
+      <c r="M15" s="17"/>
+    </row>
+    <row r="16" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="6">
-        <v>13</v>
-      </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="12">
+      <c r="D16" s="25">
+        <v>13</v>
+      </c>
+      <c r="E16" s="14"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="L15" s="10"/>
-      <c r="M15" s="18"/>
-    </row>
-    <row r="16" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C16" s="32"/>
-      <c r="D16" s="6">
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="L16" s="9"/>
+      <c r="M16" s="17"/>
+    </row>
+    <row r="17" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="24"/>
+      <c r="D17" s="25">
         <v>14</v>
       </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="12">
+      <c r="E17" s="14"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="L16" s="10"/>
-      <c r="M16" s="18"/>
-    </row>
-    <row r="17" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C17" s="30" t="s">
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="L17" s="9"/>
+      <c r="M17" s="17"/>
+    </row>
+    <row r="18" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="24">
+      <c r="D18" s="21">
         <v>15</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E18" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F18" s="7">
         <v>98.74</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G18" s="8">
         <v>0</v>
       </c>
-      <c r="H17" s="8">
+      <c r="H18" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I17" s="9" t="s">
+      <c r="I18" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J17" s="9" t="s">
+      <c r="J18" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="K17" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L17" s="20" t="s">
+      <c r="K18" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L18" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="M17" s="18"/>
-    </row>
-    <row r="18" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C18" s="30"/>
-      <c r="D18" s="6">
+      <c r="M18" s="17"/>
+    </row>
+    <row r="19" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="42"/>
+      <c r="D19" s="5">
         <v>16</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E19" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F19" s="7">
         <v>66.39</v>
       </c>
-      <c r="G18" s="9">
-        <v>1</v>
-      </c>
-      <c r="H18" s="8">
+      <c r="G19" s="8">
+        <v>1</v>
+      </c>
+      <c r="H19" s="7">
         <f t="shared" si="1"/>
         <v>66.39</v>
       </c>
-      <c r="I18" s="9" t="s">
+      <c r="I19" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J18" s="9" t="s">
+      <c r="J19" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="K18" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L18" s="20" t="s">
+      <c r="K19" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L19" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="M18" s="18"/>
-    </row>
-    <row r="19" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C19" s="30"/>
-      <c r="D19" s="6">
+      <c r="M19" s="17"/>
+    </row>
+    <row r="20" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="42"/>
+      <c r="D20" s="5">
         <v>17</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E20" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F20" s="7">
         <v>16.98</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G20" s="8">
         <v>2</v>
       </c>
-      <c r="H19" s="8">
+      <c r="H20" s="7">
         <f t="shared" si="1"/>
         <v>33.96</v>
       </c>
-      <c r="I19" s="9" t="s">
+      <c r="I20" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J19" s="9" t="s">
+      <c r="J20" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="K19" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L19" s="20" t="s">
+      <c r="K20" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L20" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="M19" s="18"/>
-    </row>
-    <row r="20" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C20" s="27" t="s">
+      <c r="M20" s="17"/>
+    </row>
+    <row r="21" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D21" s="5">
         <v>18</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E21" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="F20" s="12">
+      <c r="F21" s="11">
         <v>24.85</v>
       </c>
-      <c r="G20" s="13">
-        <v>1</v>
-      </c>
-      <c r="H20" s="12">
+      <c r="G21" s="12">
+        <v>1</v>
+      </c>
+      <c r="H21" s="11">
         <f t="shared" si="1"/>
         <v>24.85</v>
       </c>
-      <c r="I20" s="13" t="s">
+      <c r="I21" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="J20" s="13" t="s">
+      <c r="J21" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="K20" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="L20" s="20" t="s">
+      <c r="K21" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="L21" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="M20" s="18"/>
-    </row>
-    <row r="21" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C21" s="28"/>
-      <c r="D21" s="6">
+      <c r="M21" s="17"/>
+    </row>
+    <row r="22" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="43"/>
+      <c r="D22" s="5">
         <v>19</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E22" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="F21" s="12">
+      <c r="F22" s="11">
         <v>16.2</v>
       </c>
-      <c r="G21" s="13">
-        <v>1</v>
-      </c>
-      <c r="H21" s="12">
+      <c r="G22" s="12">
+        <v>1</v>
+      </c>
+      <c r="H22" s="11">
         <f t="shared" si="1"/>
         <v>16.2</v>
       </c>
-      <c r="I21" s="13" t="s">
+      <c r="I22" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="J21" s="13" t="s">
+      <c r="J22" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="K21" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="L21" s="20" t="s">
+      <c r="K22" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="L22" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="M21" s="18"/>
-    </row>
-    <row r="22" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C22" s="29"/>
-      <c r="D22" s="24">
+      <c r="M22" s="17"/>
+    </row>
+    <row r="23" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="43"/>
+      <c r="D23" s="21">
         <v>20</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="E23" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="F22" s="12">
+      <c r="F23" s="11">
         <v>22.2</v>
       </c>
-      <c r="G22" s="13">
+      <c r="G23" s="12">
         <v>0</v>
       </c>
-      <c r="H22" s="12">
+      <c r="H23" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I22" s="13" t="s">
+      <c r="I23" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="J22" s="13" t="s">
+      <c r="J23" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="K22" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="L22" s="20" t="s">
+      <c r="K23" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="L23" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="M22" s="18"/>
-    </row>
-    <row r="23" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="25" t="s">
+      <c r="M23" s="17"/>
+    </row>
+    <row r="24" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="25">
+        <v>21</v>
+      </c>
+      <c r="E24" s="6"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L24" s="19"/>
+      <c r="M24" s="17"/>
+    </row>
+    <row r="25" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="42"/>
+      <c r="D25" s="25">
+        <v>22</v>
+      </c>
+      <c r="E25" s="6"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L25" s="19"/>
+      <c r="M25" s="17"/>
+    </row>
+    <row r="26" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="42"/>
+      <c r="D26" s="25">
+        <v>23</v>
+      </c>
+      <c r="E26" s="6"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L26" s="19"/>
+      <c r="M26" s="17"/>
+    </row>
+    <row r="27" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" s="5">
+        <v>24</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="F27" s="31">
+        <v>25.93</v>
+      </c>
+      <c r="G27" s="32">
+        <v>1</v>
+      </c>
+      <c r="H27" s="11">
+        <f t="shared" si="1"/>
+        <v>25.93</v>
+      </c>
+      <c r="I27" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="J27" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="K27" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="L27" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="M27" s="17"/>
+    </row>
+    <row r="28" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="24"/>
+      <c r="D28" s="5">
+        <v>25</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F28" s="27">
+        <v>20.25</v>
+      </c>
+      <c r="G28" s="12">
+        <v>1</v>
+      </c>
+      <c r="H28" s="11">
+        <f t="shared" si="1"/>
+        <v>20.25</v>
+      </c>
+      <c r="I28" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="J28" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="K28" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="L28" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="M28" s="17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="24"/>
+      <c r="D29" s="5">
+        <v>26</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="F29" s="27">
+        <v>31.48</v>
+      </c>
+      <c r="G29" s="12">
+        <v>1</v>
+      </c>
+      <c r="H29" s="11">
+        <f t="shared" si="1"/>
+        <v>31.48</v>
+      </c>
+      <c r="I29" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="J29" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="K29" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="L29" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="M29" s="17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="24"/>
+      <c r="D30" s="5">
+        <v>27</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="F30" s="27">
+        <v>23.82</v>
+      </c>
+      <c r="G30" s="12">
+        <v>1</v>
+      </c>
+      <c r="H30" s="11">
+        <f t="shared" si="1"/>
+        <v>23.82</v>
+      </c>
+      <c r="I30" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="J30" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="K30" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="L30" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="M30" s="17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="36"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="37"/>
+      <c r="G31" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="H23" s="26">
-        <f>SUM(H3:H22)</f>
-        <v>484.68</v>
-      </c>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="2"/>
-    </row>
-    <row r="24" spans="3:13" x14ac:dyDescent="0.45">
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-    </row>
-    <row r="25" spans="3:13" x14ac:dyDescent="0.45">
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-    </row>
-    <row r="26" spans="3:13" x14ac:dyDescent="0.45">
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-    </row>
-    <row r="27" spans="3:13" x14ac:dyDescent="0.45">
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1" t="s">
+      <c r="H31" s="35">
+        <f>SUM(H4:H30)</f>
+        <v>586.16000000000008</v>
+      </c>
+      <c r="I31" s="39"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="40"/>
+      <c r="L31" s="40"/>
+      <c r="M31" s="41"/>
+    </row>
+    <row r="32" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+    </row>
+    <row r="33" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+    </row>
+    <row r="34" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+    </row>
+    <row r="35" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-    </row>
-    <row r="28" spans="3:13" x14ac:dyDescent="0.45">
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-    </row>
-    <row r="29" spans="3:13" x14ac:dyDescent="0.45">
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+    </row>
+    <row r="36" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+    </row>
+    <row r="37" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C4:C7"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C8:C11"/>
+  <mergeCells count="11">
+    <mergeCell ref="I31:M31"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C9:C12"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="L12" r:id="rId1"/>
-    <hyperlink ref="L4" r:id="rId2"/>
-    <hyperlink ref="L14" r:id="rId3" location="50785k228/=17dd33i"/>
-    <hyperlink ref="L13" r:id="rId4"/>
-    <hyperlink ref="L8" r:id="rId5"/>
-    <hyperlink ref="L6" r:id="rId6" location="3795k13/=17ddb9t"/>
-    <hyperlink ref="L5" r:id="rId7" location="50785k228/=17dd33i"/>
-    <hyperlink ref="L3" r:id="rId8" location="4067T31"/>
-    <hyperlink ref="L9" r:id="rId9"/>
-    <hyperlink ref="L10" r:id="rId10" location="50785K24"/>
-    <hyperlink ref="L7" r:id="rId11" location="50785k65/=17drpyj"/>
-    <hyperlink ref="L22" r:id="rId12" location="89965k354/=17du5gi"/>
-    <hyperlink ref="L21" r:id="rId13" location="89965k25/=17du7yu"/>
-    <hyperlink ref="L20" r:id="rId14" location="89965k571/=17du7hb"/>
-    <hyperlink ref="L17" r:id="rId15"/>
-    <hyperlink ref="L19" r:id="rId16"/>
-    <hyperlink ref="L18" r:id="rId17" location="4606k13/=17dvjpk"/>
+    <hyperlink ref="L13" r:id="rId1"/>
+    <hyperlink ref="L5" r:id="rId2"/>
+    <hyperlink ref="L15" r:id="rId3" location="50785k228/=17dd33i"/>
+    <hyperlink ref="L14" r:id="rId4"/>
+    <hyperlink ref="L9" r:id="rId5"/>
+    <hyperlink ref="L7" r:id="rId6" location="3795k13/=17ddb9t"/>
+    <hyperlink ref="L6" r:id="rId7" location="50785k228/=17dd33i"/>
+    <hyperlink ref="L4" r:id="rId8" location="4067T31"/>
+    <hyperlink ref="L10" r:id="rId9"/>
+    <hyperlink ref="L11" r:id="rId10" location="50785K24"/>
+    <hyperlink ref="L8" r:id="rId11" location="50785k65/=17drpyj"/>
+    <hyperlink ref="L23" r:id="rId12" location="89965k354/=17du5gi"/>
+    <hyperlink ref="L22" r:id="rId13" location="89965k25/=17du7yu"/>
+    <hyperlink ref="L21" r:id="rId14" location="89965k571/=17du7hb"/>
+    <hyperlink ref="L18" r:id="rId15"/>
+    <hyperlink ref="L20" r:id="rId16"/>
+    <hyperlink ref="L19" r:id="rId17" location="4606k13/=17dvjpk"/>
+    <hyperlink ref="L27" r:id="rId18" location="6362k307/=17999fj"/>
+    <hyperlink ref="L30" r:id="rId19" location="5972k129/=17e9tjt"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId18"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Massive integration of fittings order into active BOM
</commit_message>
<xml_diff>
--- a/Performance Testing/Fittings_level_tmp.xlsx
+++ b/Performance Testing/Fittings_level_tmp.xlsx
@@ -450,7 +450,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -478,6 +478,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -525,9 +531,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="8" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -576,43 +579,46 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -900,7 +906,7 @@
   <dimension ref="C1:M35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,8 +928,8 @@
     <row r="1" spans="3:13" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:13" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
       <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
@@ -948,853 +954,853 @@
       <c r="L3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="34" t="s">
+      <c r="M3" s="28" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="4" spans="3:13" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="5">
-        <v>1</v>
-      </c>
-      <c r="E4" s="25" t="s">
+      <c r="D4" s="34">
+        <v>1</v>
+      </c>
+      <c r="E4" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>10.57</v>
       </c>
-      <c r="G4" s="7">
-        <v>1</v>
-      </c>
-      <c r="H4" s="6">
+      <c r="G4" s="6">
+        <v>1</v>
+      </c>
+      <c r="H4" s="5">
         <f>F4*G4</f>
         <v>10.57</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="L4" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="M4" s="30"/>
+      <c r="K4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="M4" s="26"/>
     </row>
     <row r="5" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="34">
         <v>2</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="7">
         <v>73.180000000000007</v>
       </c>
-      <c r="G5" s="9">
-        <v>1</v>
-      </c>
-      <c r="H5" s="8">
+      <c r="G5" s="8">
+        <v>1</v>
+      </c>
+      <c r="H5" s="7">
         <f t="shared" ref="H5:H28" si="0">F5*G5</f>
         <v>73.180000000000007</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L5" s="10" t="s">
+      <c r="K5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="M5" s="31" t="s">
+      <c r="M5" s="27" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="23"/>
-      <c r="D6" s="5">
+      <c r="C6" s="33"/>
+      <c r="D6" s="34">
         <v>3</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="7">
         <v>17.399999999999999</v>
       </c>
-      <c r="G6" s="9">
-        <v>1</v>
-      </c>
-      <c r="H6" s="8">
+      <c r="G6" s="8">
+        <v>1</v>
+      </c>
+      <c r="H6" s="7">
         <f t="shared" si="0"/>
         <v>17.399999999999999</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L6" s="11" t="s">
+      <c r="K6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="M6" s="31" t="s">
+      <c r="M6" s="27" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="23"/>
-      <c r="D7" s="5">
+      <c r="C7" s="33"/>
+      <c r="D7" s="34">
         <v>4</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="7">
         <v>49.39</v>
       </c>
-      <c r="G7" s="9">
-        <v>1</v>
-      </c>
-      <c r="H7" s="8">
+      <c r="G7" s="8">
+        <v>1</v>
+      </c>
+      <c r="H7" s="7">
         <f t="shared" si="0"/>
         <v>49.39</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="K7" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L7" s="11" t="s">
+      <c r="K7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="M7" s="30"/>
+      <c r="M7" s="26"/>
     </row>
     <row r="8" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="23"/>
-      <c r="D8" s="5">
+      <c r="C8" s="33"/>
+      <c r="D8" s="34">
         <v>5</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="7">
         <v>2.54</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="8">
         <v>2</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="7">
         <f t="shared" si="0"/>
         <v>5.08</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="J8" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="K8" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L8" s="11" t="s">
+      <c r="K8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="M8" s="30"/>
+      <c r="M8" s="26"/>
     </row>
     <row r="9" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="34">
         <v>6</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <v>18.95</v>
       </c>
-      <c r="G9" s="7">
-        <v>1</v>
-      </c>
-      <c r="H9" s="6">
+      <c r="G9" s="6">
+        <v>1</v>
+      </c>
+      <c r="H9" s="5">
         <f t="shared" si="0"/>
         <v>18.95</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="I9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="7" t="s">
+      <c r="J9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="K9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="L9" s="11" t="s">
+      <c r="K9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="M9" s="30" t="s">
+      <c r="M9" s="26" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="22"/>
-      <c r="D10" s="5">
+      <c r="C10" s="30"/>
+      <c r="D10" s="34">
         <v>7</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <v>73.180000000000007</v>
       </c>
-      <c r="G10" s="7">
-        <v>1</v>
-      </c>
-      <c r="H10" s="6">
+      <c r="G10" s="6">
+        <v>1</v>
+      </c>
+      <c r="H10" s="5">
         <f t="shared" si="0"/>
         <v>73.180000000000007</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="7" t="s">
+      <c r="J10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K10" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="L10" s="10" t="s">
+      <c r="K10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="M10" s="31"/>
+      <c r="M10" s="27"/>
     </row>
     <row r="11" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="22"/>
-      <c r="D11" s="5">
+      <c r="C11" s="30"/>
+      <c r="D11" s="34">
         <v>8</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="5">
         <v>2.81</v>
       </c>
-      <c r="G11" s="7">
-        <v>1</v>
-      </c>
-      <c r="H11" s="6">
+      <c r="G11" s="6">
+        <v>1</v>
+      </c>
+      <c r="H11" s="5">
         <f t="shared" si="0"/>
         <v>2.81</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="I11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="7" t="s">
+      <c r="J11" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="K11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="L11" s="11" t="s">
+      <c r="K11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="M11" s="30"/>
+      <c r="M11" s="26"/>
     </row>
     <row r="12" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="22"/>
-      <c r="D12" s="5">
+      <c r="C12" s="30"/>
+      <c r="D12" s="34">
         <v>9</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="5">
         <v>3.69</v>
       </c>
-      <c r="G12" s="7">
-        <v>1</v>
-      </c>
-      <c r="H12" s="6">
+      <c r="G12" s="6">
+        <v>1</v>
+      </c>
+      <c r="H12" s="5">
         <f t="shared" si="0"/>
         <v>3.69</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="I12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J12" s="7" t="s">
+      <c r="J12" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="K12" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="L12" s="11" t="s">
+      <c r="K12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L12" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="M12" s="30"/>
+      <c r="M12" s="26"/>
     </row>
     <row r="13" spans="3:13" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="34">
         <v>10</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="7">
         <v>15.32</v>
       </c>
-      <c r="G13" s="9">
-        <v>1</v>
-      </c>
-      <c r="H13" s="8">
+      <c r="G13" s="8">
+        <v>1</v>
+      </c>
+      <c r="H13" s="7">
         <f t="shared" si="0"/>
         <v>15.32</v>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="I13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J13" s="15" t="s">
+      <c r="J13" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="K13" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L13" s="11" t="s">
+      <c r="K13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L13" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="M13" s="30" t="s">
+      <c r="M13" s="26" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="14" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="34">
         <v>11</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="E14" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="5">
         <v>56.31</v>
       </c>
-      <c r="G14" s="7">
-        <v>1</v>
-      </c>
-      <c r="H14" s="6">
+      <c r="G14" s="6">
+        <v>1</v>
+      </c>
+      <c r="H14" s="5">
         <f t="shared" si="0"/>
         <v>56.31</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="I14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="7" t="s">
+      <c r="J14" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="K14" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="L14" s="11" t="s">
+      <c r="K14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L14" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="M14" s="30" t="s">
+      <c r="M14" s="26" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="15" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="22"/>
-      <c r="D15" s="5">
+      <c r="C15" s="30"/>
+      <c r="D15" s="34">
         <v>12</v>
       </c>
-      <c r="E15" s="28" t="s">
+      <c r="E15" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="5">
         <v>17.399999999999999</v>
       </c>
-      <c r="G15" s="7">
-        <v>1</v>
-      </c>
-      <c r="H15" s="6">
+      <c r="G15" s="6">
+        <v>1</v>
+      </c>
+      <c r="H15" s="5">
         <f t="shared" si="0"/>
         <v>17.399999999999999</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="I15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J15" s="7" t="s">
+      <c r="J15" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="K15" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="L15" s="11" t="s">
+      <c r="K15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L15" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="M15" s="30"/>
+      <c r="M15" s="26"/>
     </row>
     <row r="16" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="12">
-        <v>13</v>
-      </c>
-      <c r="E16" s="25" t="s">
+      <c r="D16" s="11">
+        <v>13</v>
+      </c>
+      <c r="E16" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="5">
         <v>98.74</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="6">
         <v>0</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I16" s="7" t="s">
+      <c r="I16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="J16" s="7" t="s">
+      <c r="J16" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="K16" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="L16" s="11" t="s">
+      <c r="K16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L16" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="M16" s="30"/>
+      <c r="M16" s="26"/>
     </row>
     <row r="17" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="22"/>
-      <c r="D17" s="5">
+      <c r="C17" s="30"/>
+      <c r="D17" s="34">
         <v>14</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="E17" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="5">
         <v>66.39</v>
       </c>
-      <c r="G17" s="7">
-        <v>1</v>
-      </c>
-      <c r="H17" s="6">
+      <c r="G17" s="6">
+        <v>1</v>
+      </c>
+      <c r="H17" s="5">
         <f t="shared" si="0"/>
         <v>66.39</v>
       </c>
-      <c r="I17" s="7" t="s">
+      <c r="I17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J17" s="7" t="s">
+      <c r="J17" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="K17" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="L17" s="11" t="s">
+      <c r="K17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L17" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="M17" s="30"/>
+      <c r="M17" s="26"/>
     </row>
     <row r="18" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="22"/>
-      <c r="D18" s="5">
+      <c r="C18" s="30"/>
+      <c r="D18" s="34">
         <v>15</v>
       </c>
-      <c r="E18" s="25" t="s">
+      <c r="E18" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="5">
         <v>16.98</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="6">
         <v>2</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="5">
         <f t="shared" si="0"/>
         <v>33.96</v>
       </c>
-      <c r="I18" s="7" t="s">
+      <c r="I18" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="J18" s="7" t="s">
+      <c r="J18" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="K18" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="L18" s="11" t="s">
+      <c r="K18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L18" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="M18" s="30"/>
+      <c r="M18" s="26"/>
     </row>
     <row r="19" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="34">
         <v>16</v>
       </c>
-      <c r="E19" s="26" t="s">
+      <c r="E19" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="7">
         <v>24.85</v>
       </c>
-      <c r="G19" s="9">
-        <v>1</v>
-      </c>
-      <c r="H19" s="8">
+      <c r="G19" s="8">
+        <v>1</v>
+      </c>
+      <c r="H19" s="7">
         <f t="shared" si="0"/>
         <v>24.85</v>
       </c>
-      <c r="I19" s="9" t="s">
+      <c r="I19" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J19" s="9" t="s">
+      <c r="J19" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="K19" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L19" s="11" t="s">
+      <c r="K19" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L19" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="M19" s="30"/>
+      <c r="M19" s="26"/>
     </row>
     <row r="20" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="24"/>
-      <c r="D20" s="5">
+      <c r="C20" s="32"/>
+      <c r="D20" s="34">
         <v>17</v>
       </c>
-      <c r="E20" s="26" t="s">
+      <c r="E20" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="7">
         <v>16.2</v>
       </c>
-      <c r="G20" s="9">
-        <v>1</v>
-      </c>
-      <c r="H20" s="8">
+      <c r="G20" s="8">
+        <v>1</v>
+      </c>
+      <c r="H20" s="7">
         <f t="shared" si="0"/>
         <v>16.2</v>
       </c>
-      <c r="I20" s="9" t="s">
+      <c r="I20" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J20" s="9" t="s">
+      <c r="J20" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="K20" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L20" s="11" t="s">
+      <c r="K20" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L20" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="M20" s="30"/>
+      <c r="M20" s="26"/>
     </row>
     <row r="21" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="24"/>
-      <c r="D21" s="12">
+      <c r="C21" s="32"/>
+      <c r="D21" s="11">
         <v>18</v>
       </c>
-      <c r="E21" s="27" t="s">
+      <c r="E21" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F21" s="7">
         <v>22.2</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="8">
         <v>0</v>
       </c>
-      <c r="H21" s="8">
+      <c r="H21" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I21" s="9" t="s">
+      <c r="I21" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J21" s="9" t="s">
+      <c r="J21" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="K21" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L21" s="11" t="s">
+      <c r="K21" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L21" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="M21" s="30"/>
+      <c r="M21" s="26"/>
     </row>
     <row r="22" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="34">
         <v>19</v>
       </c>
-      <c r="E22" s="25" t="s">
+      <c r="E22" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="5">
         <v>131.82</v>
       </c>
-      <c r="G22" s="7">
-        <v>1</v>
-      </c>
-      <c r="H22" s="6">
+      <c r="G22" s="6">
+        <v>1</v>
+      </c>
+      <c r="H22" s="5">
         <f t="shared" si="0"/>
         <v>131.82</v>
       </c>
-      <c r="I22" s="7" t="s">
+      <c r="I22" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="J22" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="K22" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="L22" s="11" t="s">
+      <c r="J22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L22" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="M22" s="30" t="s">
+      <c r="M22" s="26" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="23" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="22"/>
-      <c r="D23" s="5">
+      <c r="C23" s="30"/>
+      <c r="D23" s="34">
         <v>20</v>
       </c>
-      <c r="E23" s="25"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="6">
+      <c r="E23" s="21"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="L23" s="11"/>
-      <c r="M23" s="30"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L23" s="10"/>
+      <c r="M23" s="26"/>
     </row>
     <row r="24" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="23" t="s">
+      <c r="C24" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="34">
         <v>21</v>
       </c>
-      <c r="E24" s="16" t="s">
+      <c r="E24" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="F24" s="29">
+      <c r="F24" s="25">
         <v>25.93</v>
       </c>
-      <c r="G24" s="17">
-        <v>1</v>
-      </c>
-      <c r="H24" s="8">
+      <c r="G24" s="16">
+        <v>1</v>
+      </c>
+      <c r="H24" s="7">
         <f t="shared" si="0"/>
         <v>25.93</v>
       </c>
-      <c r="I24" s="18" t="s">
+      <c r="I24" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="J24" s="19" t="s">
+      <c r="J24" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="K24" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L24" s="11" t="s">
+      <c r="K24" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L24" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="M24" s="30"/>
+      <c r="M24" s="26"/>
     </row>
     <row r="25" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="23"/>
-      <c r="D25" s="5">
+      <c r="C25" s="33"/>
+      <c r="D25" s="34">
         <v>22</v>
       </c>
-      <c r="E25" s="27" t="s">
+      <c r="E25" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="F25" s="8">
+      <c r="F25" s="7">
         <v>20.25</v>
       </c>
-      <c r="G25" s="9">
-        <v>1</v>
-      </c>
-      <c r="H25" s="8">
+      <c r="G25" s="8">
+        <v>1</v>
+      </c>
+      <c r="H25" s="7">
         <f t="shared" si="0"/>
         <v>20.25</v>
       </c>
-      <c r="I25" s="18" t="s">
+      <c r="I25" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="J25" s="9" t="s">
+      <c r="J25" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="K25" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L25" s="11" t="s">
+      <c r="K25" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L25" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="M25" s="30" t="s">
+      <c r="M25" s="26" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="26" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="23"/>
-      <c r="D26" s="5">
+      <c r="C26" s="33"/>
+      <c r="D26" s="34">
         <v>23</v>
       </c>
-      <c r="E26" s="27" t="s">
+      <c r="E26" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="F26" s="8">
+      <c r="F26" s="7">
         <v>2.63</v>
       </c>
-      <c r="G26" s="9">
+      <c r="G26" s="8">
         <v>3</v>
       </c>
-      <c r="H26" s="8">
+      <c r="H26" s="7">
         <f t="shared" si="0"/>
         <v>7.89</v>
       </c>
-      <c r="I26" s="18" t="s">
+      <c r="I26" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="J26" s="9" t="s">
+      <c r="J26" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="K26" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L26" s="11" t="s">
+      <c r="K26" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L26" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="M26" s="30" t="s">
+      <c r="M26" s="26" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="27" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="23"/>
-      <c r="D27" s="5">
+      <c r="C27" s="33"/>
+      <c r="D27" s="34">
         <v>24</v>
       </c>
-      <c r="E27" s="27" t="s">
+      <c r="E27" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="F27" s="8">
+      <c r="F27" s="7">
         <v>23.82</v>
       </c>
-      <c r="G27" s="9">
-        <v>1</v>
-      </c>
-      <c r="H27" s="8">
+      <c r="G27" s="8">
+        <v>1</v>
+      </c>
+      <c r="H27" s="7">
         <f t="shared" si="0"/>
         <v>23.82</v>
       </c>
-      <c r="I27" s="18" t="s">
+      <c r="I27" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="J27" s="9" t="s">
+      <c r="J27" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="K27" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L27" s="11" t="s">
+      <c r="K27" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L27" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="M27" s="30" t="s">
+      <c r="M27" s="26" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="28" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="23"/>
-      <c r="D28" s="5">
+      <c r="C28" s="33"/>
+      <c r="D28" s="34">
         <v>25</v>
       </c>
-      <c r="E28" s="27" t="s">
+      <c r="E28" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="F28" s="8">
+      <c r="F28" s="7">
         <v>153.85</v>
       </c>
-      <c r="G28" s="9">
-        <v>1</v>
-      </c>
-      <c r="H28" s="8">
+      <c r="G28" s="8">
+        <v>1</v>
+      </c>
+      <c r="H28" s="7">
         <f t="shared" si="0"/>
         <v>153.85</v>
       </c>
-      <c r="I28" s="18" t="s">
+      <c r="I28" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="J28" s="9" t="s">
+      <c r="J28" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="K28" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L28" s="11" t="s">
+      <c r="K28" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L28" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="M28" s="30" t="s">
+      <c r="M28" s="26" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="29" spans="3:13" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="13" t="s">
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="H29" s="20">
+      <c r="H29" s="19">
         <f>SUM(H4:H28)</f>
         <v>848.24</v>
       </c>
-      <c r="I29" s="33"/>
-      <c r="J29" s="33"/>
-      <c r="K29" s="33"/>
-      <c r="L29" s="33"/>
-      <c r="M29" s="33"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="29"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="29"/>
     </row>
     <row r="30" spans="3:13" x14ac:dyDescent="0.25">
       <c r="E30" s="1"/>

</xml_diff>